<commit_message>
Sprint backlog update issue 1.3 MainView
</commit_message>
<xml_diff>
--- a/doc/task06/Scrum_Team_White_V4.xlsx
+++ b/doc/task06/Scrum_Team_White_V4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hrkun\MagentaCLOUD\Weiterbildung\BFH Informatik\4. Semester\Softwareengineering and Design\ch.bfh.bti7081.s2019.white\doc\task06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yann/Documents/BFH Informatik/4 FS 2019 Module/SoED/project GIT/ch.bfh.bti7081.s2019.white/doc/task06/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454FD498-A081-4428-B8B8-F4F7D0304C29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0B4517-81A9-C147-9404-AF804FF0AE1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="24680" windowHeight="15540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="106">
   <si>
     <t>ID</t>
   </si>
@@ -209,9 +210,6 @@
     <t>HomeView fertigstellen, mit Slider, Kalendereintrag anzeigen</t>
   </si>
   <si>
-    <t>MainView mit 4 Buttons läuft, mit MainPresenter verbunden, Container für Views</t>
-  </si>
-  <si>
     <t>MoodView fertig</t>
   </si>
   <si>
@@ -348,6 +346,12 @@
   </si>
   <si>
     <t>1.15</t>
+  </si>
+  <si>
+    <t>in review</t>
+  </si>
+  <si>
+    <t>MainView mit 5 Buttons läuft, mit MainPresenter verbunden, Container für Views. Navigation lädt einzelne Views (Home, Settings, Mood, Calendar, Tips). MVP für Settings POC (proof of concept).</t>
   </si>
 </sst>
 </file>
@@ -403,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -421,14 +425,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -740,13 +741,13 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -754,7 +755,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -762,7 +763,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -770,7 +771,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -778,12 +779,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -791,7 +792,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -799,7 +800,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -825,19 +826,19 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.81640625" customWidth="1"/>
-    <col min="2" max="2" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.1796875" customWidth="1"/>
-    <col min="4" max="4" width="7.36328125" customWidth="1"/>
-    <col min="5" max="5" width="11.6328125" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="3.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -851,19 +852,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -889,7 +890,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -915,7 +916,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -941,7 +942,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -967,7 +968,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -993,7 +994,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1019,7 +1020,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1058,31 +1059,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="6.1796875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="22.36328125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="39.1796875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="19" style="7" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="8.36328125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="7.81640625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" style="7" customWidth="1"/>
-    <col min="11" max="11" width="7.1796875" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.1796875" style="7" customWidth="1"/>
-    <col min="13" max="16384" width="8.81640625" style="7"/>
+    <col min="1" max="1" width="4.83203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="39.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -1107,10 +1108,10 @@
         <v>3</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>13</v>
@@ -1119,486 +1120,479 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="9">
+    <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B2" s="7">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="D3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>1.3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2">
+        <v>4</v>
+      </c>
+      <c r="K4" s="2">
+        <v>7</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="2">
+        <v>4</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2">
+        <v>4</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>1.6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="7">
-        <v>1</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="9">
-        <v>1.2</v>
-      </c>
-      <c r="B3" s="7">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="I7" s="2">
+        <v>4</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>1.7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2">
+        <v>4</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>1.8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="2">
+        <v>4</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>1.9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2">
+        <v>4</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2">
+        <v>4</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="2">
+        <v>4</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="7">
-        <v>1</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="9">
-        <v>1.3</v>
-      </c>
-      <c r="B4" s="7">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="I13" s="2">
+        <v>4</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="2">
+        <v>4</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="2">
+        <v>4</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="7">
+      <c r="H16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="2">
         <v>4</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="9">
-        <v>1.4</v>
-      </c>
-      <c r="B5" s="7">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="7">
-        <v>4</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="B6" s="7">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="7">
-        <v>4</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="9">
-        <v>1.6</v>
-      </c>
-      <c r="B7" s="7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" s="7">
-        <v>4</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="9">
-        <v>1.7</v>
-      </c>
-      <c r="B8" s="7">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" s="7">
-        <v>4</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="9">
-        <v>1.8</v>
-      </c>
-      <c r="B9" s="7">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" s="7">
-        <v>4</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="9">
-        <v>1.9</v>
-      </c>
-      <c r="B10" s="7">
-        <v>1</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" s="7">
-        <v>4</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B11" s="7">
-        <v>1</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I11" s="7">
-        <v>4</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="7">
-        <v>1</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" s="7">
-        <v>4</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="58" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" s="7">
-        <v>4</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="7">
-        <v>1</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" s="7">
-        <v>4</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B15" s="7">
-        <v>1</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" s="7">
-        <v>4</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="58" x14ac:dyDescent="0.35">
-      <c r="A16" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B16" s="7">
-        <v>1</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I16" s="7">
-        <v>4</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D17" s="2"/>
-      <c r="I17" s="7">
+      <c r="L16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I17" s="2">
         <f>SUM(I2:I16)</f>
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1619,14 +1613,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6328125" customWidth="1"/>
-    <col min="4" max="4" width="14.36328125" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -1640,7 +1634,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1654,7 +1648,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>

</xml_diff>